<commit_message>
add discrete tree model
</commit_message>
<xml_diff>
--- a/src/example/data13_11.xlsx
+++ b/src/example/data13_11.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\16. GitHub\GaussBP\src\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\16. GitHub\FactorGraph.jl\src\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACE2622-F894-4A1B-AC6D-EF6109BD4A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DA20D1-43DD-43AA-830A-61D225F420DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3750" yWindow="810" windowWidth="21600" windowHeight="14730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4920" yWindow="1755" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jacobian" sheetId="1" r:id="rId1"/>
-    <sheet name="measurement" sheetId="3" r:id="rId2"/>
+    <sheet name="observation" sheetId="3" r:id="rId2"/>
+    <sheet name="variance" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -395,7 +396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C24"/>
     </sheetView>
   </sheetViews>
@@ -677,10 +678,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B14"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -700,120 +701,163 @@
     <col min="14" max="14" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7307636-2899-48E2-ABFA-0761AB116AAF}">
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>